<commit_message>
updates package, template and logo
- new logo, library icon and sticker
- template made remote, template xml added with update remote template path
- updates to script headers
</commit_message>
<xml_diff>
--- a/data/Flow Group.xlsx
+++ b/data/Flow Group.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr showBorderUnselectedTables="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\A249\LUCAS Base Model - Template Dev\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\stsimcbmcfs3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D03D48-8293-4CCF-9781-52DEB8B7E6DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E0AB92-486D-4997-9F87-940425C70BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5745" windowWidth="15990" windowHeight="24840" firstSheet="3" activeTab="3" xr2:uid="{7D12F415-AABC-4715-8F20-014466F1372E}"/>
+    <workbookView xWindow="6825" yWindow="3315" windowWidth="14505" windowHeight="11220" firstSheet="3" activeTab="3" xr2:uid="{7D12F415-AABC-4715-8F20-014466F1372E}"/>
   </bookViews>
   <sheets>
     <sheet name="SSim_Boolean" sheetId="3" state="hidden" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -62,64 +62,106 @@
     <t>Decay: Total</t>
   </si>
   <si>
-    <t>Emission: Total</t>
-  </si>
-  <si>
     <t>Total carbon emissions from all ecosystem components (DOM+ Biomass)</t>
   </si>
   <si>
+    <t>Net biomass increment before losses from disturbances</t>
+  </si>
+  <si>
+    <t>Transfer: Total</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Display Name</t>
+  </si>
+  <si>
+    <t>Reference Type</t>
+  </si>
+  <si>
+    <t>Data Location</t>
+  </si>
+  <si>
+    <t>Column Names</t>
+  </si>
+  <si>
+    <t>stsimsf_FlowGroup</t>
+  </si>
+  <si>
+    <t>Flow Group</t>
+  </si>
+  <si>
+    <t>Worksheet</t>
+  </si>
+  <si>
+    <t>Name,Description,Units,IsAuto</t>
+  </si>
+  <si>
+    <t>ReferenceType</t>
+  </si>
+  <si>
+    <t>Named Range</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Emission: Total Rh</t>
+  </si>
+  <si>
+    <t>LULC: Emission</t>
+  </si>
+  <si>
+    <t>LULC: Emission CH4</t>
+  </si>
+  <si>
+    <t>LULC: Emission CO</t>
+  </si>
+  <si>
+    <t>LULC: Emission CO2</t>
+  </si>
+  <si>
+    <t>LULC: Emission DOM</t>
+  </si>
+  <si>
+    <t>LULC: Emission Live</t>
+  </si>
+  <si>
+    <t>LULC: Harvest</t>
+  </si>
+  <si>
+    <t>LULC: Mortality</t>
+  </si>
+  <si>
+    <t>LULC: Transfer</t>
+  </si>
+  <si>
+    <t>Net Biome Productivity</t>
+  </si>
+  <si>
+    <t>Net Ecosystem Productivity</t>
+  </si>
+  <si>
+    <t>Net Primary Productivity</t>
+  </si>
+  <si>
+    <t>Q10 Fast Flows</t>
+  </si>
+  <si>
+    <t>Q10 Slow Flows</t>
+  </si>
+  <si>
     <t>Net Growth: Total</t>
-  </si>
-  <si>
-    <t>Net biomass increment before losses from disturbances</t>
-  </si>
-  <si>
-    <t>Transfer: Total</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Display</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Display Name</t>
-  </si>
-  <si>
-    <t>Reference Type</t>
-  </si>
-  <si>
-    <t>Data Location</t>
-  </si>
-  <si>
-    <t>Column Names</t>
-  </si>
-  <si>
-    <t>stsimsf_FlowGroup</t>
-  </si>
-  <si>
-    <t>Flow Group</t>
-  </si>
-  <si>
-    <t>Worksheet</t>
-  </si>
-  <si>
-    <t>Name,Description,Units,IsAuto</t>
-  </si>
-  <si>
-    <t>ReferenceType</t>
-  </si>
-  <si>
-    <t>Named Range</t>
-  </si>
-  <si>
-    <t>Table</t>
   </si>
 </sst>
 </file>
@@ -209,30 +251,6 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <font>
-        <b/>
-        <color rgb="FF000000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD3D3D3"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FFA9A9A9"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFA9A9A9"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -259,6 +277,30 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FFA9A9A9"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFA9A9A9"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -273,14 +315,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ADCE1ED4-4100-4AA0-8176-1AD21E400DEE}" name="Table_WorkbookManifest" displayName="Table_WorkbookManifest" ref="A1:E2" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ADCE1ED4-4100-4AA0-8176-1AD21E400DEE}" name="Table_WorkbookManifest" displayName="Table_WorkbookManifest" ref="A1:E2" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5">
   <autoFilter ref="A1:E2" xr:uid="{2FEF0386-A681-4EB7-8E0E-C846CBC4B3EC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C0AB7588-7E44-447F-9EA4-7EF7F10E29FF}" name="Name" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{DA952E82-23F1-4D89-BA61-87029F86C3B9}" name="Display Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{05505EC0-76DC-40E7-A2DC-82D45182F0FB}" name="Reference Type" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{5302663A-FCFD-4E8A-B740-2F26684ECF74}" name="Data Location" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{749C8F7D-2AAB-4B8E-89E1-BC1E0DB17362}" name="Column Names" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C0AB7588-7E44-447F-9EA4-7EF7F10E29FF}" name="Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DA952E82-23F1-4D89-BA61-87029F86C3B9}" name="Display Name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{05505EC0-76DC-40E7-A2DC-82D45182F0FB}" name="Reference Type" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{5302663A-FCFD-4E8A-B740-2F26684ECF74}" name="Data Location" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{749C8F7D-2AAB-4B8E-89E1-BC1E0DB17362}" name="Column Names" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -596,10 +638,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -607,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -615,7 +657,7 @@
         <v>-1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -639,22 +681,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -687,33 +729,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -731,19 +773,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F04C09-7013-4158-A4B8-3D6BE0E64D17}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="4" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="4" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -762,35 +804,122 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="B20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D6" xr:uid="{652DDCBB-E929-4CBF-8EEF-72A7B843B84F}"/>

</xml_diff>

<commit_message>
v1.0.14 updates (#4) merging changes by Skye
* updates to package and template library

Updated:
- transformer and datasheet naming
- age group color scheme
- transformer code clean-up

* Add remote template and remove local template

* updates package, template and logo

- new logo, library icon and sticker
- template made remote, template xml added with update remote template path
- updates to script headers
</commit_message>
<xml_diff>
--- a/data/Flow Group.xlsx
+++ b/data/Flow Group.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr showBorderUnselectedTables="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\A249\LUCAS Base Model - Template Dev\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\stsimcbmcfs3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D03D48-8293-4CCF-9781-52DEB8B7E6DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E0AB92-486D-4997-9F87-940425C70BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5745" windowWidth="15990" windowHeight="24840" firstSheet="3" activeTab="3" xr2:uid="{7D12F415-AABC-4715-8F20-014466F1372E}"/>
+    <workbookView xWindow="6825" yWindow="3315" windowWidth="14505" windowHeight="11220" firstSheet="3" activeTab="3" xr2:uid="{7D12F415-AABC-4715-8F20-014466F1372E}"/>
   </bookViews>
   <sheets>
     <sheet name="SSim_Boolean" sheetId="3" state="hidden" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -62,64 +62,106 @@
     <t>Decay: Total</t>
   </si>
   <si>
-    <t>Emission: Total</t>
-  </si>
-  <si>
     <t>Total carbon emissions from all ecosystem components (DOM+ Biomass)</t>
   </si>
   <si>
+    <t>Net biomass increment before losses from disturbances</t>
+  </si>
+  <si>
+    <t>Transfer: Total</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Display Name</t>
+  </si>
+  <si>
+    <t>Reference Type</t>
+  </si>
+  <si>
+    <t>Data Location</t>
+  </si>
+  <si>
+    <t>Column Names</t>
+  </si>
+  <si>
+    <t>stsimsf_FlowGroup</t>
+  </si>
+  <si>
+    <t>Flow Group</t>
+  </si>
+  <si>
+    <t>Worksheet</t>
+  </si>
+  <si>
+    <t>Name,Description,Units,IsAuto</t>
+  </si>
+  <si>
+    <t>ReferenceType</t>
+  </si>
+  <si>
+    <t>Named Range</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Emission: Total Rh</t>
+  </si>
+  <si>
+    <t>LULC: Emission</t>
+  </si>
+  <si>
+    <t>LULC: Emission CH4</t>
+  </si>
+  <si>
+    <t>LULC: Emission CO</t>
+  </si>
+  <si>
+    <t>LULC: Emission CO2</t>
+  </si>
+  <si>
+    <t>LULC: Emission DOM</t>
+  </si>
+  <si>
+    <t>LULC: Emission Live</t>
+  </si>
+  <si>
+    <t>LULC: Harvest</t>
+  </si>
+  <si>
+    <t>LULC: Mortality</t>
+  </si>
+  <si>
+    <t>LULC: Transfer</t>
+  </si>
+  <si>
+    <t>Net Biome Productivity</t>
+  </si>
+  <si>
+    <t>Net Ecosystem Productivity</t>
+  </si>
+  <si>
+    <t>Net Primary Productivity</t>
+  </si>
+  <si>
+    <t>Q10 Fast Flows</t>
+  </si>
+  <si>
+    <t>Q10 Slow Flows</t>
+  </si>
+  <si>
     <t>Net Growth: Total</t>
-  </si>
-  <si>
-    <t>Net biomass increment before losses from disturbances</t>
-  </si>
-  <si>
-    <t>Transfer: Total</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Display</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Display Name</t>
-  </si>
-  <si>
-    <t>Reference Type</t>
-  </si>
-  <si>
-    <t>Data Location</t>
-  </si>
-  <si>
-    <t>Column Names</t>
-  </si>
-  <si>
-    <t>stsimsf_FlowGroup</t>
-  </si>
-  <si>
-    <t>Flow Group</t>
-  </si>
-  <si>
-    <t>Worksheet</t>
-  </si>
-  <si>
-    <t>Name,Description,Units,IsAuto</t>
-  </si>
-  <si>
-    <t>ReferenceType</t>
-  </si>
-  <si>
-    <t>Named Range</t>
-  </si>
-  <si>
-    <t>Table</t>
   </si>
 </sst>
 </file>
@@ -209,30 +251,6 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <font>
-        <b/>
-        <color rgb="FF000000"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD3D3D3"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FFA9A9A9"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFA9A9A9"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -259,6 +277,30 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FFA9A9A9"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFA9A9A9"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -273,14 +315,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ADCE1ED4-4100-4AA0-8176-1AD21E400DEE}" name="Table_WorkbookManifest" displayName="Table_WorkbookManifest" ref="A1:E2" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ADCE1ED4-4100-4AA0-8176-1AD21E400DEE}" name="Table_WorkbookManifest" displayName="Table_WorkbookManifest" ref="A1:E2" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5">
   <autoFilter ref="A1:E2" xr:uid="{2FEF0386-A681-4EB7-8E0E-C846CBC4B3EC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C0AB7588-7E44-447F-9EA4-7EF7F10E29FF}" name="Name" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{DA952E82-23F1-4D89-BA61-87029F86C3B9}" name="Display Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{05505EC0-76DC-40E7-A2DC-82D45182F0FB}" name="Reference Type" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{5302663A-FCFD-4E8A-B740-2F26684ECF74}" name="Data Location" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{749C8F7D-2AAB-4B8E-89E1-BC1E0DB17362}" name="Column Names" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C0AB7588-7E44-447F-9EA4-7EF7F10E29FF}" name="Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DA952E82-23F1-4D89-BA61-87029F86C3B9}" name="Display Name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{05505EC0-76DC-40E7-A2DC-82D45182F0FB}" name="Reference Type" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{5302663A-FCFD-4E8A-B740-2F26684ECF74}" name="Data Location" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{749C8F7D-2AAB-4B8E-89E1-BC1E0DB17362}" name="Column Names" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -596,10 +638,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -607,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -615,7 +657,7 @@
         <v>-1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -639,22 +681,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -687,33 +729,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -731,19 +773,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F04C09-7013-4158-A4B8-3D6BE0E64D17}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="4" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="4" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -762,35 +804,122 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="B20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D6" xr:uid="{652DDCBB-E929-4CBF-8EEF-72A7B843B84F}"/>

</xml_diff>

<commit_message>
updated to flow types; conus template lib added
- updates to data inputs related to flow type
- update to flow-pathways script to simplify flow types
- updates to cbmcfs3 example library
</commit_message>
<xml_diff>
--- a/data/Flow Group.xlsx
+++ b/data/Flow Group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\stsimcbmcfs3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E0AB92-486D-4997-9F87-940425C70BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06ED4249-3C08-4A78-9498-BF8561FAFDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6825" yWindow="3315" windowWidth="14505" windowHeight="11220" firstSheet="3" activeTab="3" xr2:uid="{7D12F415-AABC-4715-8F20-014466F1372E}"/>
+    <workbookView xWindow="6390" yWindow="2400" windowWidth="14610" windowHeight="11565" firstSheet="3" activeTab="3" xr2:uid="{7D12F415-AABC-4715-8F20-014466F1372E}"/>
   </bookViews>
   <sheets>
     <sheet name="SSim_Boolean" sheetId="3" state="hidden" r:id="rId1"/>
@@ -18,10 +18,14 @@
     <sheet name="Workbook Manifest" sheetId="4" state="hidden" r:id="rId3"/>
     <sheet name="Flow Group" sheetId="2" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Flow Group'!$A$1:$D$6</definedName>
     <definedName name="Range_ManifestReferenceTypes">ManifestReferenceTypes!$A$2:$A$4</definedName>
     <definedName name="Range_SSim_Boolean">SSim_Boolean!$B$2:$B$3</definedName>
+    <definedName name="Range_stsimsf_FlowGroup">[1]stsimsf_FlowGroup!$B$2:$B$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -161,7 +165,7 @@
     <t>Q10 Slow Flows</t>
   </si>
   <si>
-    <t>Net Growth: Total</t>
+    <t>Net Growth Forest: Total</t>
   </si>
 </sst>
 </file>
@@ -233,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -243,6 +247,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -312,6 +319,233 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="stsimsf_FlowType"/>
+      <sheetName val="stsimsf_FlowGroup"/>
+      <sheetName val="ManifestReferenceTypes"/>
+      <sheetName val="Workbook Manifest"/>
+      <sheetName val="Flow Type-Group Membership"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Biomass Turnover: Coarse Roots -&gt; AG Fast [Type]</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Biomass Turnover: Coarse Roots -&gt; BG Fast [Type]</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Biomass Turnover: Fine Roots -&gt; AG Very Fast [Type]</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Biomass Turnover: Fine Roots -&gt; BG Very Fast [Type]</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>Biomass Turnover: Foliage -&gt; AG Very Fast [Type]</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Biomass Turnover: Merchantable -&gt; Snag Stems [Type]</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Biomass Turnover: Other Wood -&gt; AG Fast [Type]</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Biomass Turnover: Other Wood -&gt; Snag Branches [Type]</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Biomass Turnover: Total</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>Decay: AG Fast -&gt; AG Slow [Type]</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>Decay: AG Medium -&gt; AG Slow [Type]</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>Decay: AG Very Fast -&gt; AG Slow [Type]</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>Decay: BG Fast -&gt; BG Slow [Type]</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>Decay: BG Very Fast -&gt; BG Slow [Type]</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>Decay: Snag Branch -&gt; AG Slow [Type]</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>Decay: Snag Stem -&gt; AG Slow [Type]</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18" t="str">
+            <v>Decay: Total</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19" t="str">
+            <v>Emission: AG Fast -&gt; Atmosphere [Type]</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v>Emission: AG Medium -&gt; Atmosphere [Type]</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>Emission: AG Slow -&gt; Atmosphere [Type]</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>Emission: AG Very Fast -&gt; Atmosphere [Type]</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>Emission: BG Fast -&gt; Atmosphere [Type]</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>Emission: BG Slow -&gt; Atmosphere [Type]</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>Emission: BG Very Fast -&gt; Atmosphere [Type]</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>Emission: Snag Branch -&gt; Atmosphere [Type]</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>Emission: Snag Stem -&gt; Atmosphere [Type]</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>Emission: Total</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29" t="str">
+            <v>LULC: Emission [Type]</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30" t="str">
+            <v>LULC: Harvest [Type]</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31" t="str">
+            <v>LULC: Mortality [Type]</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32" t="str">
+            <v>LULC: Transfer [Type]</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33" t="str">
+            <v>Net Growth: Atmosphere -&gt; Coarse Roots [Type]</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>Net Growth: Atmosphere -&gt; Fine Roots [Type]</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35" t="str">
+            <v>Net Growth: Atmosphere -&gt; Foliage [Type]</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36" t="str">
+            <v>Net Growth: Atmosphere -&gt; Merchantable [Type]</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37" t="str">
+            <v>Net Growth: Atmosphere -&gt; Other Wood [Type]</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38" t="str">
+            <v>Net Growth: Total</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39" t="str">
+            <v>Transfer: AG Slow -&gt; BG Slow [Type]</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40" t="str">
+            <v>Transfer: Snag Branch -&gt; AG Fast [Type]</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41" t="str">
+            <v>Transfer: Snag Stem -&gt; AG Medium [Type]</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42" t="str">
+            <v>Transfer: Total</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -776,8 +1010,8 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +1124,7 @@
       <c r="B15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B16" t="s">
@@ -923,9 +1157,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D6" xr:uid="{652DDCBB-E929-4CBF-8EEF-72A7B843B84F}"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You must choose 'IsAuto' from the supplied list of items." sqref="D2:D1048576" xr:uid="{09D559D2-E0FA-4CC7-A651-A0A98CB3125E}">
       <formula1>Range_SSim_Boolean</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You must choose 'FlowGroupID' from the supplied list of items." sqref="A16" xr:uid="{D60FB26F-4411-4A5E-85E9-13506768FF89}">
+      <formula1>Range_stsimsf_FlowGroup</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>